<commit_message>
import excel sheet purpose
import excel sheet purpose
</commit_message>
<xml_diff>
--- a/assets/subcategoryimportfiles/grocerycategoryfile.xlsx
+++ b/assets/subcategoryimportfiles/grocerycategoryfile.xlsx
@@ -16,44 +16,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
   <si>
     <t>sno</t>
   </si>
   <si>
-    <t>Status</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>https://i.ytimg.com/vi/NtaX9WJMgvk/hqdefault.jpg</t>
-  </si>
-  <si>
-    <t>https://i.stack.imgur.com/4AffV.png</t>
-  </si>
-  <si>
-    <t>https://static.pexels.com/photos/39517/rose-flower-blossom-bloom-39517.jpeg</t>
-  </si>
-  <si>
-    <t>https://static.pexels.com/photos/36764/marguerite-daisy-beautiful-beauty.jpg</t>
-  </si>
-  <si>
-    <t>https://static.pexels.com/photos/36753/flower-purple-lical-blosso.jpg</t>
-  </si>
-  <si>
-    <t>http://images.all-free-download.com/images/graphiclarge/hd_pictures_of_beautiful_flowers_05_166896.jpg</t>
-  </si>
-  <si>
-    <t>Sku code</t>
-  </si>
-  <si>
-    <t>Other Unique code</t>
-  </si>
-  <si>
-    <t>Product name</t>
-  </si>
-  <si>
     <t>price</t>
   </si>
   <si>
@@ -63,122 +30,141 @@
     <t>Qty</t>
   </si>
   <si>
-    <t>Meta keywords</t>
-  </si>
-  <si>
-    <t>Meta title</t>
-  </si>
-  <si>
-    <t>Product description</t>
-  </si>
-  <si>
-    <t>otherunique</t>
-  </si>
-  <si>
-    <t>999</t>
-  </si>
-  <si>
-    <t>50</t>
-  </si>
-  <si>
-    <t>metakeyword</t>
-  </si>
-  <si>
-    <t>meta tile</t>
-  </si>
-  <si>
-    <t>description</t>
-  </si>
-  <si>
-    <t>Product specifications name</t>
-  </si>
-  <si>
-    <t>Product specifications value</t>
-  </si>
-  <si>
-    <t>ram,hardisk</t>
-  </si>
-  <si>
-    <t>4gb,500gb</t>
-  </si>
-  <si>
-    <t>55555</t>
-  </si>
-  <si>
-    <t>Offers</t>
-  </si>
-  <si>
-    <t>Discount</t>
-  </si>
-  <si>
-    <t>Subitem</t>
-  </si>
-  <si>
-    <t>Product image1</t>
-  </si>
-  <si>
-    <t>Product image2</t>
-  </si>
-  <si>
-    <t>Product image3</t>
-  </si>
-  <si>
-    <t>Product image4</t>
-  </si>
-  <si>
-    <t>Product image5</t>
-  </si>
-  <si>
-    <t>Product image6</t>
-  </si>
-  <si>
-    <t>Product image7</t>
-  </si>
-  <si>
-    <t>Product image8</t>
-  </si>
-  <si>
-    <t>Product image9</t>
-  </si>
-  <si>
-    <t>Product image10</t>
-  </si>
-  <si>
-    <t>Product image11</t>
-  </si>
-  <si>
-    <t>Product image12</t>
-  </si>
-  <si>
-    <t>12</t>
-  </si>
-  <si>
-    <t>10</t>
-  </si>
-  <si>
-    <t>subitem</t>
-  </si>
-  <si>
     <t>Brand</t>
   </si>
   <si>
-    <t>Sizes</t>
-  </si>
-  <si>
-    <t>puma</t>
-  </si>
-  <si>
-    <t>12,20</t>
-  </si>
-  <si>
-    <t>fruites</t>
+    <t>product Name</t>
+  </si>
+  <si>
+    <t>Highlights</t>
+  </si>
+  <si>
+    <t>Description1</t>
+  </si>
+  <si>
+    <t>image1</t>
+  </si>
+  <si>
+    <t>Description2</t>
+  </si>
+  <si>
+    <t>image2</t>
+  </si>
+  <si>
+    <t>Description3</t>
+  </si>
+  <si>
+    <t>image3</t>
+  </si>
+  <si>
+    <t>Description4</t>
+  </si>
+  <si>
+    <t>image4</t>
+  </si>
+  <si>
+    <t>Warranty Summary</t>
+  </si>
+  <si>
+    <t>Warranty Type</t>
+  </si>
+  <si>
+    <t>Service Type</t>
+  </si>
+  <si>
+    <t>Return Policy</t>
+  </si>
+  <si>
+    <t>Product Code</t>
+  </si>
+  <si>
+    <t>Image1</t>
+  </si>
+  <si>
+    <t>Image2</t>
+  </si>
+  <si>
+    <t>Image3</t>
+  </si>
+  <si>
+    <t>Image4</t>
+  </si>
+  <si>
+    <t>Image5</t>
+  </si>
+  <si>
+    <t>Image6</t>
+  </si>
+  <si>
+    <t>Image7</t>
+  </si>
+  <si>
+    <t>Image8</t>
+  </si>
+  <si>
+    <t>46</t>
+  </si>
+  <si>
+    <t>SAMSUNG Guru Music 2 B310</t>
+  </si>
+  <si>
+    <t>2 inch NA Display
+800 mAh Battery
+0 0 0 208MHz Processor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Brand Warranty of 1 Year Available for Mobile and 6 Months for Accessories
+</t>
+  </si>
+  <si>
+    <t>repair</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7 days return policy
+</t>
+  </si>
+  <si>
+    <t>SAMSUNG</t>
+  </si>
+  <si>
+    <t>SAMSUNG Guru Music 2 B310 black</t>
+  </si>
+  <si>
+    <t>Ingredients</t>
+  </si>
+  <si>
+    <t>Key Features</t>
+  </si>
+  <si>
+    <t>Unit</t>
+  </si>
+  <si>
+    <t>Packaging Type</t>
+  </si>
+  <si>
+    <t>Disclaimer</t>
+  </si>
+  <si>
+    <t>in</t>
+  </si>
+  <si>
+    <t>key</t>
+  </si>
+  <si>
+    <t>unit</t>
+  </si>
+  <si>
+    <t>package</t>
+  </si>
+  <si>
+    <t>dis</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -188,7 +174,35 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF2F2F2F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -207,7 +221,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -215,19 +229,67 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Accent1" xfId="1" builtinId="29"/>
+    <cellStyle name="Heading 3" xfId="1" builtinId="18"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -520,10 +582,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AD2"/>
+  <dimension ref="A1:AG2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" topLeftCell="X1" workbookViewId="0">
+      <selection activeCell="AH2" sqref="AH2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -537,203 +599,195 @@
     <col min="7" max="7" width="8.140625" style="1" customWidth="1"/>
     <col min="8" max="8" width="8.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10.42578125" style="1" customWidth="1"/>
-    <col min="10" max="10" width="17.140625" style="1" customWidth="1"/>
-    <col min="11" max="11" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="17.140625" style="1" customWidth="1"/>
     <col min="12" max="12" width="6.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="18.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="14" max="16" width="18.5703125" style="1" customWidth="1"/>
     <col min="17" max="17" width="20.7109375" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="33.28515625" customWidth="1"/>
     <col min="19" max="19" width="48" customWidth="1"/>
-    <col min="20" max="30" width="48.28515625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="48.28515625" bestFit="1" customWidth="1"/>
+    <col min="21" max="25" width="48.28515625" customWidth="1"/>
+    <col min="26" max="27" width="7.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" s="3" customFormat="1">
+    <row r="1" spans="1:33" s="5" customFormat="1" ht="15.75" thickBot="1">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="K1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="M1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="N1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="R1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="S1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="T1" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="V1" t="s">
+        <v>37</v>
+      </c>
+      <c r="W1" t="s">
+        <v>38</v>
+      </c>
+      <c r="X1" t="s">
+        <v>39</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>40</v>
+      </c>
+      <c r="Z1" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="AA1" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="AB1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="AC1" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="AD1" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="AE1" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="AF1" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="AG1" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:33">
+      <c r="A2" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="C2" s="8">
+        <v>1953.85</v>
+      </c>
+      <c r="D2" s="9">
+        <v>1699</v>
+      </c>
+      <c r="E2" s="10">
+        <v>100</v>
+      </c>
+      <c r="F2" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="I1" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="L1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="M1" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="N1" s="3" t="s">
+      <c r="G2" s="11"/>
+      <c r="I2" s="11"/>
+      <c r="K2" s="11"/>
+      <c r="M2" s="11"/>
+      <c r="O2" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="O1" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="P1" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="Q1" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="R1" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="S1" s="2" t="s">
+      <c r="Q2" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="T1" s="2" t="s">
+      <c r="R2" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="U1" s="2" t="s">
+      <c r="S2" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="V1" s="2" t="s">
+      <c r="T2" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="W1" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="X1" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="Y1" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="Z1" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="AA1" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="AB1" s="2" t="s">
+      <c r="U2" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="AC1" s="2" t="s">
+      <c r="V2" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="AD1" s="2" t="s">
+      <c r="W2" s="13" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="2" spans="1:30">
-      <c r="A2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G2" s="1" t="s">
+      <c r="X2" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="Y2" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="I2" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="M2" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="O2" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="P2" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>26</v>
-      </c>
-      <c r="R2" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="S2" t="s">
-        <v>3</v>
-      </c>
-      <c r="T2" t="s">
-        <v>4</v>
-      </c>
-      <c r="U2" t="s">
-        <v>5</v>
-      </c>
-      <c r="V2" t="s">
-        <v>6</v>
-      </c>
-      <c r="W2" t="s">
-        <v>7</v>
-      </c>
-      <c r="X2" t="s">
-        <v>8</v>
-      </c>
-      <c r="Y2" t="s">
-        <v>3</v>
-      </c>
-      <c r="Z2" t="s">
-        <v>3</v>
-      </c>
-      <c r="AA2" t="s">
-        <v>3</v>
-      </c>
-      <c r="AB2" t="s">
-        <v>3</v>
-      </c>
-      <c r="AC2" t="s">
-        <v>3</v>
-      </c>
-      <c r="AD2" t="s">
-        <v>3</v>
-      </c>
+      <c r="Z2" s="13"/>
+      <c r="AA2" s="13"/>
+      <c r="AB2" s="13"/>
+      <c r="AC2" s="13"/>
+      <c r="AD2" s="13"/>
+      <c r="AE2" s="13"/>
+      <c r="AF2" s="13"/>
+      <c r="AG2" s="13"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="Q1:XFD1 A1:N1">
+  <conditionalFormatting sqref="Z1:XFD1 A1:N1 Q1:U1">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AH1:XFD1 H1:N1 A1">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min" val="0"/>

</xml_diff>